<commit_message>
Added DTO in Search Service
</commit_message>
<xml_diff>
--- a/game-manager-service/assets/GameMovies.xlsx
+++ b/game-manager-service/assets/GameMovies.xlsx
@@ -259,7 +259,7 @@
     </font>
     <font>
       <b val="true"/>
-      <sz val="12"/>
+      <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="0"/>
@@ -352,8 +352,8 @@
   </sheetPr>
   <dimension ref="A1:AA1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I14" activeCellId="0" sqref="I14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -829,7 +829,7 @@
       <c r="C13" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" s="5" t="s">
         <v>53</v>
       </c>
       <c r="E13" s="1" t="s">

</xml_diff>

<commit_message>
Edited Game Manager Service
</commit_message>
<xml_diff>
--- a/game-manager-service/assets/GameMovies.xlsx
+++ b/game-manager-service/assets/GameMovies.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="52">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -34,9 +34,6 @@
     <t xml:space="preserve">Genre</t>
   </si>
   <si>
-    <t xml:space="preserve">Tag</t>
-  </si>
-  <si>
     <t xml:space="preserve">Level</t>
   </si>
   <si>
@@ -64,16 +61,13 @@
     <t xml:space="preserve">Drama</t>
   </si>
   <si>
-    <t xml:space="preserve">null</t>
-  </si>
-  <si>
     <t xml:space="preserve">easy</t>
   </si>
   <si>
     <t xml:space="preserve">https://lh3.googleusercontent.com/-M-l-fj3erPw/UxPopIR3qVI/AAAAAAAAABM/mw7ROBKAezY/w530-h531-n-rw/NOOBIELOGO.jpg</t>
   </si>
   <si>
-    <t xml:space="preserve">This Quiz has 5 questions.+The questions are of difficulty level “Easy”.+Total time given for this quiz is 5 minutes.+Once a Option is selected, it can’t be changed.</t>
+    <t xml:space="preserve">Each Question will have Multiple Options.+Among them only one Option is Correct.+Player can\'t move to Next Question until an Option has been Selected.+Player can change Selected Option.+After timeout Game-Window will be automatically closed.</t>
   </si>
   <si>
     <t xml:space="preserve">Movie Pros</t>
@@ -88,9 +82,6 @@
     <t xml:space="preserve">http://static1.squarespace.com/static/562169c4e4b013a54e869666/t/572144837c65e4ed40cc9b61/1529012403727/?format=1500w</t>
   </si>
   <si>
-    <t xml:space="preserve">This Quiz has 6 questions.+The questions are of difficulty level “Medium”.+Total time given for this quiz is 6 minutes.+Once a Option is selected, it can’t be changed.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Movie Legends</t>
   </si>
   <si>
@@ -103,18 +94,12 @@
     <t xml:space="preserve">https://www.logolynx.com/images/logolynx/2a/2a52c0210d4f09ae93ccd2a9f7b6807c.jpeg</t>
   </si>
   <si>
-    <t xml:space="preserve">This Quiz has 7 questions.+The questions are of difficulty level “Hard”.+Total time given for this quiz is 7 minutes.+Once a Option is selected, it can’t be changed.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Action Aware</t>
   </si>
   <si>
     <t xml:space="preserve">https://previews.123rf.com/images/iqoncept/iqoncept1109/iqoncept110900015/10465601-the-word-action-as-a-3d-illustration-with-an-arrow-hitting-a-target-bullseye-in-the-letter-o-represe.jpg</t>
   </si>
   <si>
-    <t xml:space="preserve">This Quiz has 7 questions.+The questions are of difficulty level “Easy”.+Total time given for this quiz is 7 minutes.+Once a Option is selected, it can’t be changed.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Comedy Canvas</t>
   </si>
   <si>
@@ -122,9 +107,6 @@
   </si>
   <si>
     <t xml:space="preserve">https://www.brunel.ac.uk/research/Images/CCSRimage.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">This Quiz has 7 questions.+The questions are of difficulty level “Medium”.+Total time given for this quiz is 7 minutes.+Once a Option is selected, it can’t be changed.</t>
   </si>
   <si>
     <t xml:space="preserve">Romance Birds</t>
@@ -350,10 +332,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AA1048576"/>
+  <dimension ref="A1:Z1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K13" activeCellId="0" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -362,13 +344,13 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="21.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="19.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="23.76"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="18.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="15.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="25.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="27.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="195.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="32.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="11" style="1" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="15.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="25.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="15.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="31.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="19.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="10" style="1" width="14.43"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -399,9 +381,7 @@
       <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
-        <v>9</v>
-      </c>
+      <c r="K1" s="2"/>
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
       <c r="N1" s="2"/>
@@ -417,39 +397,36 @@
       <c r="X1" s="2"/>
       <c r="Y1" s="2"/>
       <c r="Z1" s="2"/>
-      <c r="AA1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2" s="2" t="n">
+      <c r="G2" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="I2" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="J2" s="2" t="n">
-        <v>300</v>
-      </c>
+      <c r="H2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="K2" s="2"/>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
@@ -465,39 +442,36 @@
       <c r="X2" s="2"/>
       <c r="Y2" s="2"/>
       <c r="Z2" s="2"/>
-      <c r="AA2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="2" t="s">
+      <c r="F3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H3" s="2" t="n">
+      <c r="G3" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="I3" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="J3" s="2" t="n">
-        <v>360</v>
-      </c>
+      <c r="H3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" s="2" t="n">
+        <v>150</v>
+      </c>
+      <c r="K3" s="2"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
@@ -513,39 +487,36 @@
       <c r="X3" s="2"/>
       <c r="Y3" s="2"/>
       <c r="Z3" s="2"/>
-      <c r="AA3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="H4" s="2" t="n">
-        <v>7</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="J4" s="2" t="n">
-        <v>420</v>
-      </c>
+      <c r="G4" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4" s="2" t="n">
+        <v>210</v>
+      </c>
+      <c r="K4" s="2"/>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
@@ -561,334 +532,303 @@
       <c r="X4" s="2"/>
       <c r="Y4" s="2"/>
       <c r="Z4" s="2"/>
-      <c r="AA4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="H5" s="2" t="n">
-        <v>7</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="J5" s="2" t="n">
-        <v>420</v>
+        <v>13</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I5" s="2" t="n">
+        <v>150</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="H6" s="2" t="n">
-        <v>7</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="J6" s="2" t="n">
-        <v>420</v>
+        <v>18</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G6" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I6" s="2" t="n">
+        <v>180</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="H7" s="2" t="n">
-        <v>7</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="J7" s="2" t="n">
-        <v>420</v>
+        <v>22</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G7" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I7" s="2" t="n">
+        <v>210</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="H8" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="I8" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="J8" s="2" t="n">
-        <v>420</v>
+        <v>13</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G8" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I8" s="2" t="n">
+        <v>150</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="H9" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="I9" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="J9" s="2" t="n">
-        <v>420</v>
+        <v>18</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I9" s="2" t="n">
+        <v>180</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="30.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="H10" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="I10" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="J10" s="2" t="n">
-        <v>420</v>
+        <v>22</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G10" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I10" s="2" t="n">
+        <v>210</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="E11" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E11" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="H11" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="I11" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="J11" s="2" t="n">
-        <v>420</v>
+      <c r="F11" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G11" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I11" s="2" t="n">
+        <v>150</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="H12" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="I12" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="J12" s="2" t="n">
-        <v>420</v>
+        <v>22</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G12" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I12" s="2" t="n">
+        <v>180</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="H13" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="I13" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="J13" s="2" t="n">
-        <v>420</v>
+        <v>48</v>
+      </c>
+      <c r="G13" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I13" s="2" t="n">
+        <v>210</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="H14" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="I14" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="J14" s="1" t="n">
-        <v>420</v>
+        <v>51</v>
+      </c>
+      <c r="G14" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I14" s="2" t="n">
+        <v>150</v>
       </c>
     </row>
     <row r="1048576" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1" display="https://lh3.googleusercontent.com/-M-l-fj3erPw/UxPopIR3qVI/AAAAAAAAABM/mw7ROBKAezY/w530-h531-n-rw/NOOBIELOGO.jpg"/>
-    <hyperlink ref="G3" r:id="rId2" display="http://static1.squarespace.com/static/562169c4e4b013a54e869666/t/572144837c65e4ed40cc9b61/1529012403727/?format=1500w"/>
-    <hyperlink ref="G4" r:id="rId3" display="https://www.logolynx.com/images/logolynx/2a/2a52c0210d4f09ae93ccd2a9f7b6807c.jpeg"/>
+    <hyperlink ref="F2" r:id="rId1" display="https://lh3.googleusercontent.com/-M-l-fj3erPw/UxPopIR3qVI/AAAAAAAAABM/mw7ROBKAezY/w530-h531-n-rw/NOOBIELOGO.jpg"/>
+    <hyperlink ref="F3" r:id="rId2" display="http://static1.squarespace.com/static/562169c4e4b013a54e869666/t/572144837c65e4ed40cc9b61/1529012403727/?format=1500w"/>
+    <hyperlink ref="F4" r:id="rId3" display="https://www.logolynx.com/images/logolynx/2a/2a52c0210d4f09ae93ccd2a9f7b6807c.jpeg"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Assets of game manager is updated
</commit_message>
<xml_diff>
--- a/game-manager-service/assets/GameMovies.xlsx
+++ b/game-manager-service/assets/GameMovies.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="79">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -64,7 +64,7 @@
     <t xml:space="preserve">easy</t>
   </si>
   <si>
-    <t xml:space="preserve">https://previews.123rf.com/images/iqoncept/iqoncept1109/iqoncept110900015/10465601-the-word-action-as-a-3d-illustration-with-an-arrow-hitting-a-target-bullseye-in-the-letter-o-represe.jpg</t>
+    <t xml:space="preserve">https://wallpapercave.com/wp/wp2044878.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Each Question will have Multiple Options.+Among them only one Option is Correct.+Player can\'t move to Next Question until an Option has been Selected.+Player can change Selected Option.+After timeout Game-Window will be automatically closed.</t>
@@ -79,7 +79,7 @@
     <t xml:space="preserve">hard</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.brunel.ac.uk/research/Images/CCSRimage.jpg</t>
+    <t xml:space="preserve">https://www.wallpapersbyte.com/wp-content/uploads/2015/06/Smiles-Smileys-Smile-Yellow-Balls-WallpapersByte-com-1280x1024.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Thriller Seekers</t>
@@ -103,13 +103,37 @@
     <t xml:space="preserve">https://vignette.wikia.nocookie.net/central/images/a/ab/Romance.png/revision/latest?cb=20171028034947</t>
   </si>
   <si>
+    <t xml:space="preserve">Hostory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Historical</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://images8.alphacoders.com/717/thumb-350-717747.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ActionMania</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://wallpapercave.com/wp/wp2044883.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Comic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://wallpapercave.com/wp/wp2312775.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://images2.alphacoders.com/845/thumb-1920-84502.jpg</t>
+  </si>
+  <si>
     <t xml:space="preserve">Drama Classics</t>
   </si>
   <si>
     <t xml:space="preserve">Drama</t>
   </si>
   <si>
-    <t xml:space="preserve">https://static1.squarespace.com/static/55bffa14e4b0536353951cf6/t/5bec7ee621c67c90311e07df/1549313840943/</t>
+    <t xml:space="preserve">https://images.alphacoders.com/637/thumb-350-637541.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Documentary Deck</t>
@@ -130,7 +154,7 @@
     <t xml:space="preserve">Reality &amp; Talk Shows</t>
   </si>
   <si>
-    <t xml:space="preserve">https://i.ytimg.com/vi/35zv9khFQs0/maxresdefault.jpg</t>
+    <t xml:space="preserve">https://images4.alphacoders.com/807/thumb-1920-807881.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">SiciFi Solvers</t>
@@ -145,13 +169,31 @@
     <t xml:space="preserve">Thriller Scholars</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.tes.com/sites/default/files/styles/news_article_hero/public/introducing-secondary-students-new-historical-periods.png?itok=tTrH9LCx</t>
+    <t xml:space="preserve">https://wallpapercave.com/wp/msi4htu.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://www.nwave.com/wp-content/uploads/2018/09/nWave_FD_ARCHEOPTERYX.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://images5.alphacoders.com/807/thumb-1920-807880.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://images.alphacoders.com/252/thumb-1920-252233.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://images4.alphacoders.com/845/thumb-1920-84504.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://images4.alphacoders.com/132/thumb-1920-132008.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://images7.alphacoders.com/910/thumb-350-910103.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Reality Resolvers</t>
   </si>
   <si>
-    <t xml:space="preserve">https://upload.wikimedia.org/wikipedia/de/a/ac/Reality_Show_Logo.jpg</t>
+    <t xml:space="preserve">https://images.alphacoders.com/818/thumb-1920-818873.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Captial Pros</t>
@@ -169,13 +211,52 @@
     <t xml:space="preserve">http://practicemock.com/blog/wp-content-uploads/2017/12/Countries-Capitals-770x515.png</t>
   </si>
   <si>
-    <t xml:space="preserve">World Leaders</t>
+    <t xml:space="preserve">Captial Master</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://1.bp.blogspot.com/-AgMuCdpzs6I/U6BfePHb02I/AAAAAAAAElM/EvxRhsbsf3o/s1600/world-leaders.gif</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://images4.alphacoders.com/217/thumb-350-217624.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       Capitals</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://images6.alphacoders.com/377/thumb-350-377219.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://images4.alphacoders.com/551/thumb-350-551555.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Languages</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://images7.alphacoders.com/567/thumb-350-567990.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://images7.alphacoders.com/679/thumb-350-679140.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://images4.alphacoders.com/202/thumb-350-202478.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Presidents</t>
   </si>
   <si>
-    <t xml:space="preserve">https://1.bp.blogspot.com/-AgMuCdpzs6I/U6BfePHb02I/AAAAAAAAElM/EvxRhsbsf3o/s1600/world-leaders.gif</t>
+    <t xml:space="preserve">https://images3.alphacoders.com/566/thumb-350-566269.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://images8.alphacoders.com/790/thumb-350-790642.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://images5.alphacoders.com/905/thumb-350-905759.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://images6.alphacoders.com/681/thumb-350-681347.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://images5.alphacoders.com/905/thumb-1920-905759.jpg</t>
   </si>
 </sst>
 </file>
@@ -185,7 +266,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="12">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -241,11 +322,30 @@
     </font>
     <font>
       <b val="true"/>
-      <sz val="9"/>
+      <sz val="13"/>
+      <name val="arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="13"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="0"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="13"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="0"/>
     </font>
   </fonts>
   <fills count="2">
@@ -290,7 +390,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -319,6 +419,22 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -336,10 +452,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Z1048576"/>
+  <dimension ref="A1:Z36"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
+      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -519,20 +635,20 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="3" t="s">
         <v>27</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="3" t="s">
         <v>28</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>29</v>
@@ -540,221 +656,835 @@
       <c r="G6" s="3" t="n">
         <v>10</v>
       </c>
-      <c r="H6" s="5" t="s">
+      <c r="H6" s="7" t="s">
         <v>15</v>
       </c>
       <c r="I6" s="3" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G7" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="I7" s="3" t="n">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G8" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="I8" s="3" t="n">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="3"/>
+      <c r="B9" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G9" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="I9" s="3" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G10" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="I10" s="3" t="n">
         <v>200</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G7" s="3" t="n">
-        <v>10</v>
-      </c>
-      <c r="H7" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="I7" s="3" t="n">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G8" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="H8" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="I8" s="1" t="n">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="30.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="G9" s="3" t="n">
-        <v>10</v>
-      </c>
-      <c r="H9" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="I9" s="3" t="n">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="G10" s="3" t="n">
-        <v>10</v>
-      </c>
-      <c r="H10" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="I10" s="3" t="n">
-        <v>250</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G11" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="I11" s="3" t="n">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="E11" s="1" t="s">
+      <c r="B12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="I12" s="1" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="30.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E13" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="F13" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="G13" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="I13" s="3" t="n">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G14" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="I14" s="3" t="n">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B15" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G15" s="3" t="n">
+        <v>15</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="I15" s="3" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B16" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="G11" s="3" t="n">
-        <v>10</v>
-      </c>
-      <c r="H11" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="I11" s="3" t="n">
+      <c r="E16" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="G16" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="H16" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="I16" s="3" t="n">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B17" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="G17" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="H17" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="I17" s="3" t="n">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B18" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="G18" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="H18" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="I18" s="3" t="n">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B19" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="G19" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="H19" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="I19" s="3" t="n">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B20" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="G20" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="H20" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="I20" s="3" t="n">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G21" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="H21" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="I21" s="3" t="n">
         <v>200</v>
       </c>
     </row>
-    <row r="12" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E12" s="2" t="s">
+    <row r="22" s="2" customFormat="true" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="E22" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="F12" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="G12" s="2" t="n">
-        <v>15</v>
-      </c>
-      <c r="H12" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="I12" s="2" t="n">
+      <c r="F22" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="G22" s="8" t="n">
+        <v>15</v>
+      </c>
+      <c r="H22" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="I22" s="8" t="n">
         <v>300</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="E13" s="1" t="s">
+    <row r="23" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E23" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F13" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="G13" s="1" t="n">
-        <v>15</v>
-      </c>
-      <c r="H13" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="I13" s="1" t="n">
+      <c r="F23" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G23" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="H23" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="I23" s="1" t="n">
         <v>450</v>
       </c>
     </row>
-    <row r="1048573" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="24" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B24" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G24" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="H24" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="I24" s="1" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B25" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G25" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="H25" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="I25" s="1" t="n">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B26" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="G26" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="H26" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="I26" s="1" t="n">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B27" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="G27" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="H27" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="I27" s="1" t="n">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B28" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G28" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="H28" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="I28" s="1" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B29" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G29" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="H29" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="I29" s="1" t="n">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B30" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G30" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="H30" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="I30" s="1" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B31" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G31" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="H31" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="I31" s="1" t="n">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B32" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G32" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="H32" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="I32" s="1" t="n">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B33" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G33" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="H33" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="I33" s="1" t="n">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B34" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="G34" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="H34" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="I34" s="1" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B35" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="G35" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="H35" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="I35" s="1" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B36" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G36" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="H36" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="I36" s="1" t="n">
+        <v>450</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F2" r:id="rId1" display="https://wallpapercave.com/wp/wp2044878.jpg"/>
+    <hyperlink ref="F3" r:id="rId2" display="https://www.wallpapersbyte.com/wp-content/uploads/2015/06/Smiles-Smileys-Smile-Yellow-Balls-WallpapersByte-com-1280x1024.jpg"/>
+    <hyperlink ref="F7" r:id="rId3" display="https://wallpapercave.com/wp/wp2044883.jpg"/>
+    <hyperlink ref="F8" r:id="rId4" display="https://wallpapercave.com/wp/wp2312775.jpg"/>
+    <hyperlink ref="F9" r:id="rId5" display="https://images2.alphacoders.com/845/thumb-1920-84502.jpg"/>
+    <hyperlink ref="F10" r:id="rId6" display="https://images.alphacoders.com/637/thumb-350-637541.jpg"/>
+    <hyperlink ref="F12" r:id="rId7" display="https://images4.alphacoders.com/807/thumb-1920-807881.jpg"/>
+    <hyperlink ref="F14" r:id="rId8" display="https://wallpapercave.com/wp/msi4htu.jpg"/>
+    <hyperlink ref="F18" r:id="rId9" display="https://images4.alphacoders.com/845/thumb-1920-84504.jpg"/>
+    <hyperlink ref="F19" r:id="rId10" display="https://images4.alphacoders.com/132/thumb-1920-132008.jpg"/>
+    <hyperlink ref="F20" r:id="rId11" display="https://images7.alphacoders.com/910/thumb-350-910103.jpg"/>
+    <hyperlink ref="F21" r:id="rId12" display="https://images.alphacoders.com/818/thumb-1920-818873.jpg"/>
+    <hyperlink ref="F24" r:id="rId13" display="https://images4.alphacoders.com/217/thumb-350-217624.jpg"/>
+    <hyperlink ref="F36" r:id="rId14" display="https://images5.alphacoders.com/905/thumb-1920-905759.jpg"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>